<commit_message>
Regenerated SPARQL validation reports for packages F02 and F05 after fixing CM (version 2.1.2-alpha.5), to avoid error reports caused by a new line character in the name of the field IV.2.7.1.
</commit_message>
<xml_diff>
--- a/mappings/package_F05/transformation/conceptual_mappings.xlsx
+++ b/mappings/package_F05/transformation/conceptual_mappings.xlsx
@@ -54,7 +54,7 @@
     <t>Mapping Version</t>
   </si>
   <si>
-    <t>2.1.2-alpha.1</t>
+    <t>2.1.2-alpha.5</t>
   </si>
   <si>
     <r>
@@ -5820,8 +5820,7 @@
     <t>IV.2.7.1</t>
   </si>
   <si>
-    <t>Public Opening
-(Date/Time)</t>
+    <t>Public Opening (Date/Time)</t>
   </si>
   <si>
     <t>BT-132</t>

</xml_diff>